<commit_message>
impr: code-gen: 优化Entity模板，其他Fix refactor: 多语言文件移至src\Modules\XXX\Gardener.XXX\DB Locale
</commit_message>
<xml_diff>
--- a/src/Gardener.Entry/wwwroot/DB Locale/Sys/Sys_Code_Gen.xlsx
+++ b/src/Gardener.Entry/wwwroot/DB Locale/Sys/Sys_Code_Gen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\GitHub\Github-Fork\Gardener\src\Gardener.Entry\bin\Debug\net6.0\codeGen\Sys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\GitHub\Github-Fork\Gardener\src\Gardener.Entry\wwwroot\DB Locale\Sys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F650B08-D65C-43DC-82BC-61C6AE225D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87316E87-A898-4633-8FB0-E56EFB267D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>ValueEN</t>
   </si>
   <si>
-    <t>ValueCN</t>
-  </si>
-  <si>
     <t>Sys_Code_Gen</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>表前缀</t>
+  </si>
+  <si>
+    <t>ValueCH</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -524,287 +526,287 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>